<commit_message>
add rnn pavel excel results, scripts
</commit_message>
<xml_diff>
--- a/new-dataset/models/diff_weights/method-debug-dima/hnn-mse-sigma-0-nb_plays#-25-units#-25-__state__--1.xlsx
+++ b/new-dataset/models/diff_weights/method-debug-dima/hnn-mse-sigma-0-nb_plays#-25-units#-25-__state__--1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zxchen/fu/feng/new-dataset/models/diff_weights/method-debug-dima/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A019D2E-05E5-E14A-A05C-483179EB449E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C79558-C84D-5649-AD3E-F6C5768D8536}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="460" windowWidth="27880" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nb_plays-50-pred" sheetId="1" r:id="rId1"/>
@@ -289,3338 +289,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="zh-CN"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'nb_plays-50-pred'!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>outputs</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'nb_plays-50-pred'!$C$2:$C$401</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="400"/>
-                <c:pt idx="0">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.6280000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9.6280000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.6280000000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9.6280000000000001</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>10.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>10.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>9.6280000000000001</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>9.6280000000000001</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>10.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>10.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>9.6280000000000001</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>9.6280000000000001</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>10.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>10.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>9.6280000000000001</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>9.6280000000000001</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>10.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>10.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>9.6280000000000001</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>9.6280000000000001</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>10.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>10.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>9.6280000000000001</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>9.6280000000000001</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>10.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>10.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>10.019</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>9.7839999999999989</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>11.297000000000001</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>11.297000000000001</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>10.019</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>9.7839999999999989</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>11.297000000000001</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>11.297000000000001</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>10.019</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>9.7839999999999989</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>11.297000000000001</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>11.297000000000001</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>10.019</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>9.7839999999999989</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>11.297000000000001</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>11.297000000000001</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>10.019</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>9.7839999999999989</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>11.297000000000001</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>11.297000000000001</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>10.019</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>9.7839999999999989</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>11.297000000000001</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>11.297000000000001</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>10.019</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>9.7839999999999989</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>11.297000000000001</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>11.297000000000001</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>10.019</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>9.85</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>11.917</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>11.917</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>10.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>9.947000000000001</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>11.917</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>11.917</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>10.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>9.947000000000001</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>11.917</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>11.917</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>10.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>9.947000000000001</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>11.917</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>11.917</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>10.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>9.947000000000001</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>11.917</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>11.917</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>10.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>9.947000000000001</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>11.917</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>11.917</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>10.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>9.947000000000001</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>11.917</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>11.917</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>10.311999999999999</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>9.947000000000001</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>10.723000000000001</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>10.176</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>10.723000000000001</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>10.176</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>10.723000000000001</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>10.176</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>10.723000000000001</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>10.176</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>10.723000000000001</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>10.176</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>10.723000000000001</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>10.176</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>10.723000000000001</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>10.176</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>9.4909999999999997</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>14.454000000000001</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>11.476000000000001</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>10.518000000000001</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>14.454000000000001</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>9.4909999999999997</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>14.454000000000001</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>11.476000000000001</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>10.518000000000001</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>14.454000000000001</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>9.4909999999999997</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>14.454000000000001</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>11.476000000000001</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>10.518000000000001</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>14.454000000000001</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>9.4909999999999997</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>14.454000000000001</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>11.476000000000001</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>10.518000000000001</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>14.454000000000001</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>9.4909999999999997</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>14.454000000000001</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>11.476000000000001</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>10.518000000000001</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>14.454000000000001</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>9.4909999999999997</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>14.454000000000001</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>11.476000000000001</c:v>
-                </c:pt>
-                <c:pt idx="240">
-                  <c:v>10.518000000000001</c:v>
-                </c:pt>
-                <c:pt idx="241">
-                  <c:v>14.454000000000001</c:v>
-                </c:pt>
-                <c:pt idx="242">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="243">
-                  <c:v>9.4909999999999997</c:v>
-                </c:pt>
-                <c:pt idx="244">
-                  <c:v>14.454000000000001</c:v>
-                </c:pt>
-                <c:pt idx="245">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="246">
-                  <c:v>11.476000000000001</c:v>
-                </c:pt>
-                <c:pt idx="247">
-                  <c:v>10.518000000000001</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>14.454000000000001</c:v>
-                </c:pt>
-                <c:pt idx="249">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="250">
-                  <c:v>9.7189999999999994</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>17.376000000000001</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>11.164</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>17.376000000000001</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>9.7189999999999994</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>17.376000000000001</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>11.164</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>17.376000000000001</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>9.7189999999999994</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>17.376000000000001</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>11.164</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>17.376000000000001</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>9.7189999999999994</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>17.376000000000001</c:v>
-                </c:pt>
-                <c:pt idx="273">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="274">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="275">
-                  <c:v>11.164</c:v>
-                </c:pt>
-                <c:pt idx="276">
-                  <c:v>17.376000000000001</c:v>
-                </c:pt>
-                <c:pt idx="277">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="278">
-                  <c:v>9.7189999999999994</c:v>
-                </c:pt>
-                <c:pt idx="279">
-                  <c:v>17.376000000000001</c:v>
-                </c:pt>
-                <c:pt idx="280">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="281">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="282">
-                  <c:v>11.164</c:v>
-                </c:pt>
-                <c:pt idx="283">
-                  <c:v>17.376000000000001</c:v>
-                </c:pt>
-                <c:pt idx="284">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="285">
-                  <c:v>9.7189999999999994</c:v>
-                </c:pt>
-                <c:pt idx="286">
-                  <c:v>17.376000000000001</c:v>
-                </c:pt>
-                <c:pt idx="287">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="288">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="289">
-                  <c:v>11.164</c:v>
-                </c:pt>
-                <c:pt idx="290">
-                  <c:v>17.376000000000001</c:v>
-                </c:pt>
-                <c:pt idx="291">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="292">
-                  <c:v>9.7189999999999994</c:v>
-                </c:pt>
-                <c:pt idx="293">
-                  <c:v>17.376000000000001</c:v>
-                </c:pt>
-                <c:pt idx="294">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="295">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="296">
-                  <c:v>11.164</c:v>
-                </c:pt>
-                <c:pt idx="297">
-                  <c:v>17.376000000000001</c:v>
-                </c:pt>
-                <c:pt idx="298">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="299">
-                  <c:v>9.7189999999999994</c:v>
-                </c:pt>
-                <c:pt idx="300">
-                  <c:v>47.906999999999996</c:v>
-                </c:pt>
-                <c:pt idx="301">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="302">
-                  <c:v>28.396999999999998</c:v>
-                </c:pt>
-                <c:pt idx="303">
-                  <c:v>17.832999999999998</c:v>
-                </c:pt>
-                <c:pt idx="304">
-                  <c:v>47.906999999999996</c:v>
-                </c:pt>
-                <c:pt idx="305">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="306">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="307">
-                  <c:v>47.906999999999996</c:v>
-                </c:pt>
-                <c:pt idx="308">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="309">
-                  <c:v>28.396999999999998</c:v>
-                </c:pt>
-                <c:pt idx="310">
-                  <c:v>17.832999999999998</c:v>
-                </c:pt>
-                <c:pt idx="311">
-                  <c:v>47.906999999999996</c:v>
-                </c:pt>
-                <c:pt idx="312">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="313">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="314">
-                  <c:v>47.906999999999996</c:v>
-                </c:pt>
-                <c:pt idx="315">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="316">
-                  <c:v>28.396999999999998</c:v>
-                </c:pt>
-                <c:pt idx="317">
-                  <c:v>17.832999999999998</c:v>
-                </c:pt>
-                <c:pt idx="318">
-                  <c:v>47.906999999999996</c:v>
-                </c:pt>
-                <c:pt idx="319">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="320">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="321">
-                  <c:v>47.906999999999996</c:v>
-                </c:pt>
-                <c:pt idx="322">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="323">
-                  <c:v>28.396999999999998</c:v>
-                </c:pt>
-                <c:pt idx="324">
-                  <c:v>17.832999999999998</c:v>
-                </c:pt>
-                <c:pt idx="325">
-                  <c:v>47.906999999999996</c:v>
-                </c:pt>
-                <c:pt idx="326">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="327">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="328">
-                  <c:v>47.906999999999996</c:v>
-                </c:pt>
-                <c:pt idx="329">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="330">
-                  <c:v>28.396999999999998</c:v>
-                </c:pt>
-                <c:pt idx="331">
-                  <c:v>17.832999999999998</c:v>
-                </c:pt>
-                <c:pt idx="332">
-                  <c:v>47.906999999999996</c:v>
-                </c:pt>
-                <c:pt idx="333">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="334">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="335">
-                  <c:v>47.906999999999996</c:v>
-                </c:pt>
-                <c:pt idx="336">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="337">
-                  <c:v>28.396999999999998</c:v>
-                </c:pt>
-                <c:pt idx="338">
-                  <c:v>17.832999999999998</c:v>
-                </c:pt>
-                <c:pt idx="339">
-                  <c:v>47.906999999999996</c:v>
-                </c:pt>
-                <c:pt idx="340">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="341">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="342">
-                  <c:v>47.906999999999996</c:v>
-                </c:pt>
-                <c:pt idx="343">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="344">
-                  <c:v>28.396999999999998</c:v>
-                </c:pt>
-                <c:pt idx="345">
-                  <c:v>17.832999999999998</c:v>
-                </c:pt>
-                <c:pt idx="346">
-                  <c:v>47.906999999999996</c:v>
-                </c:pt>
-                <c:pt idx="347">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="348">
-                  <c:v>12.868</c:v>
-                </c:pt>
-                <c:pt idx="349">
-                  <c:v>47.906999999999996</c:v>
-                </c:pt>
-                <c:pt idx="350">
-                  <c:v>9.3539999999999992</c:v>
-                </c:pt>
-                <c:pt idx="351">
-                  <c:v>60.226000000000013</c:v>
-                </c:pt>
-                <c:pt idx="352">
-                  <c:v>31.774000000000001</c:v>
-                </c:pt>
-                <c:pt idx="353">
-                  <c:v>109.504</c:v>
-                </c:pt>
-                <c:pt idx="354">
-                  <c:v>13.691000000000001</c:v>
-                </c:pt>
-                <c:pt idx="355">
-                  <c:v>24.254000000000001</c:v>
-                </c:pt>
-                <c:pt idx="356">
-                  <c:v>109.504</c:v>
-                </c:pt>
-                <c:pt idx="357">
-                  <c:v>13.691000000000001</c:v>
-                </c:pt>
-                <c:pt idx="358">
-                  <c:v>62.895000000000003</c:v>
-                </c:pt>
-                <c:pt idx="359">
-                  <c:v>34.442999999999998</c:v>
-                </c:pt>
-                <c:pt idx="360">
-                  <c:v>109.504</c:v>
-                </c:pt>
-                <c:pt idx="361">
-                  <c:v>13.691000000000001</c:v>
-                </c:pt>
-                <c:pt idx="362">
-                  <c:v>24.254000000000001</c:v>
-                </c:pt>
-                <c:pt idx="363">
-                  <c:v>109.504</c:v>
-                </c:pt>
-                <c:pt idx="364">
-                  <c:v>13.691000000000001</c:v>
-                </c:pt>
-                <c:pt idx="365">
-                  <c:v>62.895000000000003</c:v>
-                </c:pt>
-                <c:pt idx="366">
-                  <c:v>34.442999999999998</c:v>
-                </c:pt>
-                <c:pt idx="367">
-                  <c:v>109.504</c:v>
-                </c:pt>
-                <c:pt idx="368">
-                  <c:v>13.691000000000001</c:v>
-                </c:pt>
-                <c:pt idx="369">
-                  <c:v>24.254000000000001</c:v>
-                </c:pt>
-                <c:pt idx="370">
-                  <c:v>109.504</c:v>
-                </c:pt>
-                <c:pt idx="371">
-                  <c:v>13.691000000000001</c:v>
-                </c:pt>
-                <c:pt idx="372">
-                  <c:v>62.895000000000003</c:v>
-                </c:pt>
-                <c:pt idx="373">
-                  <c:v>34.442999999999998</c:v>
-                </c:pt>
-                <c:pt idx="374">
-                  <c:v>109.504</c:v>
-                </c:pt>
-                <c:pt idx="375">
-                  <c:v>13.691000000000001</c:v>
-                </c:pt>
-                <c:pt idx="376">
-                  <c:v>24.254000000000001</c:v>
-                </c:pt>
-                <c:pt idx="377">
-                  <c:v>109.504</c:v>
-                </c:pt>
-                <c:pt idx="378">
-                  <c:v>13.691000000000001</c:v>
-                </c:pt>
-                <c:pt idx="379">
-                  <c:v>62.895000000000003</c:v>
-                </c:pt>
-                <c:pt idx="380">
-                  <c:v>34.442999999999998</c:v>
-                </c:pt>
-                <c:pt idx="381">
-                  <c:v>109.504</c:v>
-                </c:pt>
-                <c:pt idx="382">
-                  <c:v>13.691000000000001</c:v>
-                </c:pt>
-                <c:pt idx="383">
-                  <c:v>24.254000000000001</c:v>
-                </c:pt>
-                <c:pt idx="384">
-                  <c:v>109.504</c:v>
-                </c:pt>
-                <c:pt idx="385">
-                  <c:v>13.691000000000001</c:v>
-                </c:pt>
-                <c:pt idx="386">
-                  <c:v>62.895000000000003</c:v>
-                </c:pt>
-                <c:pt idx="387">
-                  <c:v>34.442999999999998</c:v>
-                </c:pt>
-                <c:pt idx="388">
-                  <c:v>109.504</c:v>
-                </c:pt>
-                <c:pt idx="389">
-                  <c:v>13.691000000000001</c:v>
-                </c:pt>
-                <c:pt idx="390">
-                  <c:v>24.254000000000001</c:v>
-                </c:pt>
-                <c:pt idx="391">
-                  <c:v>109.504</c:v>
-                </c:pt>
-                <c:pt idx="392">
-                  <c:v>13.691000000000001</c:v>
-                </c:pt>
-                <c:pt idx="393">
-                  <c:v>62.895000000000003</c:v>
-                </c:pt>
-                <c:pt idx="394">
-                  <c:v>34.442999999999998</c:v>
-                </c:pt>
-                <c:pt idx="395">
-                  <c:v>109.504</c:v>
-                </c:pt>
-                <c:pt idx="396">
-                  <c:v>13.691000000000001</c:v>
-                </c:pt>
-                <c:pt idx="397">
-                  <c:v>24.254000000000001</c:v>
-                </c:pt>
-                <c:pt idx="398">
-                  <c:v>109.504</c:v>
-                </c:pt>
-                <c:pt idx="399">
-                  <c:v>13.691000000000001</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D71B-764F-BA8E-8B7840D13606}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'nb_plays-50-pred'!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>nb_plays-50-units-50-__activation__-elu-__nb_plays__-25-__units__-25-ensemble-1=predictions</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'nb_plays-50-pred'!$D$2:$D$401</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="400"/>
-                <c:pt idx="0">
-                  <c:v>-2.766</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.633</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.109</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.2869999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.2869999999999999</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.109</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.2869999999999999</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.5310000000000001</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.4980000000000002</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.109</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.2869999999999999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3.2869999999999999</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4.109</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.2869999999999999</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.5310000000000001</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.4980000000000002</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>4.109</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3.2869999999999999</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.2869999999999999</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>4.109</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3.2869999999999999</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3.5310000000000001</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3.4980000000000002</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>4.109</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3.2869999999999999</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3.2869999999999999</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>4.109</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>3.2869999999999999</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>3.5310000000000001</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3.4980000000000002</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>4.109</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>3.2869999999999999</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>3.2869999999999999</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>4.109</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>3.2869999999999999</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>3.5310000000000001</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>3.4980000000000002</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>4.109</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>3.2869999999999999</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>3.2869999999999999</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>4.109</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>3.2869999999999999</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>3.5310000000000001</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>3.4980000000000002</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>4.109</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>3.2869999999999999</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>3.2869999999999999</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>4.109</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>3.2869999999999999</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>3.8620000000000001</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>3.6739999999999999</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>6.5070000000000006</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>4.7249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>4.7249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>6.5070000000000006</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>4.7249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>5.3</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>5.1120000000000001</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>6.5070000000000006</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>4.7249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>4.7249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>6.5070000000000006</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>4.7249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>5.3</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>5.1120000000000001</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>6.5070000000000006</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>4.7249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>4.7249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>6.5070000000000006</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>4.7249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="71">
-                  <c:v>5.3</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>5.1120000000000001</c:v>
-                </c:pt>
-                <c:pt idx="73">
-                  <c:v>6.5070000000000006</c:v>
-                </c:pt>
-                <c:pt idx="74">
-                  <c:v>4.7249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="75">
-                  <c:v>4.7249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="76">
-                  <c:v>6.5070000000000006</c:v>
-                </c:pt>
-                <c:pt idx="77">
-                  <c:v>4.7249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="78">
-                  <c:v>5.3</c:v>
-                </c:pt>
-                <c:pt idx="79">
-                  <c:v>5.1120000000000001</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>6.5070000000000006</c:v>
-                </c:pt>
-                <c:pt idx="81">
-                  <c:v>4.7249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="82">
-                  <c:v>4.7249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="83">
-                  <c:v>6.5070000000000006</c:v>
-                </c:pt>
-                <c:pt idx="84">
-                  <c:v>4.7249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="85">
-                  <c:v>5.3</c:v>
-                </c:pt>
-                <c:pt idx="86">
-                  <c:v>5.1120000000000001</c:v>
-                </c:pt>
-                <c:pt idx="87">
-                  <c:v>6.5070000000000006</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>4.7249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="89">
-                  <c:v>4.7249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="90">
-                  <c:v>6.5070000000000006</c:v>
-                </c:pt>
-                <c:pt idx="91">
-                  <c:v>4.7249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="92">
-                  <c:v>5.3</c:v>
-                </c:pt>
-                <c:pt idx="93">
-                  <c:v>5.1120000000000001</c:v>
-                </c:pt>
-                <c:pt idx="94">
-                  <c:v>6.5070000000000006</c:v>
-                </c:pt>
-                <c:pt idx="95">
-                  <c:v>4.7249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>4.7249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="97">
-                  <c:v>6.5070000000000006</c:v>
-                </c:pt>
-                <c:pt idx="98">
-                  <c:v>4.7249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="99">
-                  <c:v>5.3</c:v>
-                </c:pt>
-                <c:pt idx="100">
-                  <c:v>5.157</c:v>
-                </c:pt>
-                <c:pt idx="101">
-                  <c:v>7.7649999999999997</c:v>
-                </c:pt>
-                <c:pt idx="102">
-                  <c:v>5.3550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="103">
-                  <c:v>5.3550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>7.7649999999999997</c:v>
-                </c:pt>
-                <c:pt idx="105">
-                  <c:v>5.3550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="106">
-                  <c:v>6.1760000000000002</c:v>
-                </c:pt>
-                <c:pt idx="107">
-                  <c:v>5.91</c:v>
-                </c:pt>
-                <c:pt idx="108">
-                  <c:v>7.7649999999999997</c:v>
-                </c:pt>
-                <c:pt idx="109">
-                  <c:v>5.3550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="110">
-                  <c:v>5.3550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="111">
-                  <c:v>7.7649999999999997</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>5.3550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="113">
-                  <c:v>6.1760000000000002</c:v>
-                </c:pt>
-                <c:pt idx="114">
-                  <c:v>5.91</c:v>
-                </c:pt>
-                <c:pt idx="115">
-                  <c:v>7.7649999999999997</c:v>
-                </c:pt>
-                <c:pt idx="116">
-                  <c:v>5.3550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="117">
-                  <c:v>5.3550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="118">
-                  <c:v>7.7649999999999997</c:v>
-                </c:pt>
-                <c:pt idx="119">
-                  <c:v>5.3550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>6.1760000000000002</c:v>
-                </c:pt>
-                <c:pt idx="121">
-                  <c:v>5.91</c:v>
-                </c:pt>
-                <c:pt idx="122">
-                  <c:v>7.7649999999999997</c:v>
-                </c:pt>
-                <c:pt idx="123">
-                  <c:v>5.3550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="124">
-                  <c:v>5.3550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="125">
-                  <c:v>7.7649999999999997</c:v>
-                </c:pt>
-                <c:pt idx="126">
-                  <c:v>5.3550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="127">
-                  <c:v>6.1760000000000002</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>5.91</c:v>
-                </c:pt>
-                <c:pt idx="129">
-                  <c:v>7.7649999999999997</c:v>
-                </c:pt>
-                <c:pt idx="130">
-                  <c:v>5.3550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="131">
-                  <c:v>5.3550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="132">
-                  <c:v>7.7649999999999997</c:v>
-                </c:pt>
-                <c:pt idx="133">
-                  <c:v>5.3550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="134">
-                  <c:v>6.1760000000000002</c:v>
-                </c:pt>
-                <c:pt idx="135">
-                  <c:v>5.91</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>7.7649999999999997</c:v>
-                </c:pt>
-                <c:pt idx="137">
-                  <c:v>5.3550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="138">
-                  <c:v>5.3550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="139">
-                  <c:v>7.7649999999999997</c:v>
-                </c:pt>
-                <c:pt idx="140">
-                  <c:v>5.3550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="141">
-                  <c:v>6.1760000000000002</c:v>
-                </c:pt>
-                <c:pt idx="142">
-                  <c:v>5.91</c:v>
-                </c:pt>
-                <c:pt idx="143">
-                  <c:v>7.7649999999999997</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>5.3550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="145">
-                  <c:v>5.3550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="146">
-                  <c:v>7.7649999999999997</c:v>
-                </c:pt>
-                <c:pt idx="147">
-                  <c:v>5.3550000000000004</c:v>
-                </c:pt>
-                <c:pt idx="148">
-                  <c:v>6.1760000000000002</c:v>
-                </c:pt>
-                <c:pt idx="149">
-                  <c:v>5.91</c:v>
-                </c:pt>
-                <c:pt idx="150">
-                  <c:v>9.4640000000000004</c:v>
-                </c:pt>
-                <c:pt idx="151">
-                  <c:v>6.0489999999999986</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>6.0870000000000006</c:v>
-                </c:pt>
-                <c:pt idx="153">
-                  <c:v>9.4640000000000004</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>6.0489999999999986</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>7.2670000000000003</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>6.8490000000000002</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>9.4640000000000004</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>6.0489999999999986</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>6.0870000000000006</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>9.4640000000000004</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>6.0489999999999986</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>7.2670000000000003</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>6.8490000000000002</c:v>
-                </c:pt>
-                <c:pt idx="164">
-                  <c:v>9.4640000000000004</c:v>
-                </c:pt>
-                <c:pt idx="165">
-                  <c:v>6.0489999999999986</c:v>
-                </c:pt>
-                <c:pt idx="166">
-                  <c:v>6.0870000000000006</c:v>
-                </c:pt>
-                <c:pt idx="167">
-                  <c:v>9.4640000000000004</c:v>
-                </c:pt>
-                <c:pt idx="168">
-                  <c:v>6.0489999999999986</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>7.2670000000000003</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>6.8490000000000002</c:v>
-                </c:pt>
-                <c:pt idx="171">
-                  <c:v>9.4640000000000004</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>6.0489999999999986</c:v>
-                </c:pt>
-                <c:pt idx="173">
-                  <c:v>6.0870000000000006</c:v>
-                </c:pt>
-                <c:pt idx="174">
-                  <c:v>9.4640000000000004</c:v>
-                </c:pt>
-                <c:pt idx="175">
-                  <c:v>6.0489999999999986</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>7.2670000000000003</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>6.8490000000000002</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>9.4640000000000004</c:v>
-                </c:pt>
-                <c:pt idx="179">
-                  <c:v>6.0489999999999986</c:v>
-                </c:pt>
-                <c:pt idx="180">
-                  <c:v>6.0870000000000006</c:v>
-                </c:pt>
-                <c:pt idx="181">
-                  <c:v>9.4640000000000004</c:v>
-                </c:pt>
-                <c:pt idx="182">
-                  <c:v>6.0489999999999986</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>7.2670000000000003</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>6.8490000000000002</c:v>
-                </c:pt>
-                <c:pt idx="185">
-                  <c:v>9.4640000000000004</c:v>
-                </c:pt>
-                <c:pt idx="186">
-                  <c:v>6.0489999999999986</c:v>
-                </c:pt>
-                <c:pt idx="187">
-                  <c:v>6.0870000000000006</c:v>
-                </c:pt>
-                <c:pt idx="188">
-                  <c:v>9.4640000000000004</c:v>
-                </c:pt>
-                <c:pt idx="189">
-                  <c:v>6.0489999999999986</c:v>
-                </c:pt>
-                <c:pt idx="190">
-                  <c:v>7.2670000000000003</c:v>
-                </c:pt>
-                <c:pt idx="191">
-                  <c:v>6.8490000000000002</c:v>
-                </c:pt>
-                <c:pt idx="192">
-                  <c:v>9.4640000000000004</c:v>
-                </c:pt>
-                <c:pt idx="193">
-                  <c:v>6.0489999999999986</c:v>
-                </c:pt>
-                <c:pt idx="194">
-                  <c:v>6.0870000000000006</c:v>
-                </c:pt>
-                <c:pt idx="195">
-                  <c:v>9.4640000000000004</c:v>
-                </c:pt>
-                <c:pt idx="196">
-                  <c:v>6.0489999999999986</c:v>
-                </c:pt>
-                <c:pt idx="197">
-                  <c:v>7.2670000000000003</c:v>
-                </c:pt>
-                <c:pt idx="198">
-                  <c:v>6.8490000000000002</c:v>
-                </c:pt>
-                <c:pt idx="199">
-                  <c:v>9.4640000000000004</c:v>
-                </c:pt>
-                <c:pt idx="200">
-                  <c:v>6.0489999999999986</c:v>
-                </c:pt>
-                <c:pt idx="201">
-                  <c:v>6.194</c:v>
-                </c:pt>
-                <c:pt idx="202">
-                  <c:v>11.896000000000001</c:v>
-                </c:pt>
-                <c:pt idx="203">
-                  <c:v>6.8039999999999994</c:v>
-                </c:pt>
-                <c:pt idx="204">
-                  <c:v>8.7670000000000012</c:v>
-                </c:pt>
-                <c:pt idx="205">
-                  <c:v>8.0489999999999995</c:v>
-                </c:pt>
-                <c:pt idx="206">
-                  <c:v>11.896000000000001</c:v>
-                </c:pt>
-                <c:pt idx="207">
-                  <c:v>6.8039999999999994</c:v>
-                </c:pt>
-                <c:pt idx="208">
-                  <c:v>6.9480000000000004</c:v>
-                </c:pt>
-                <c:pt idx="209">
-                  <c:v>11.896000000000001</c:v>
-                </c:pt>
-                <c:pt idx="210">
-                  <c:v>6.8039999999999994</c:v>
-                </c:pt>
-                <c:pt idx="211">
-                  <c:v>8.7670000000000012</c:v>
-                </c:pt>
-                <c:pt idx="212">
-                  <c:v>8.0489999999999995</c:v>
-                </c:pt>
-                <c:pt idx="213">
-                  <c:v>11.896000000000001</c:v>
-                </c:pt>
-                <c:pt idx="214">
-                  <c:v>6.8039999999999994</c:v>
-                </c:pt>
-                <c:pt idx="215">
-                  <c:v>6.9480000000000004</c:v>
-                </c:pt>
-                <c:pt idx="216">
-                  <c:v>11.896000000000001</c:v>
-                </c:pt>
-                <c:pt idx="217">
-                  <c:v>6.8039999999999994</c:v>
-                </c:pt>
-                <c:pt idx="218">
-                  <c:v>8.7670000000000012</c:v>
-                </c:pt>
-                <c:pt idx="219">
-                  <c:v>8.0489999999999995</c:v>
-                </c:pt>
-                <c:pt idx="220">
-                  <c:v>11.896000000000001</c:v>
-                </c:pt>
-                <c:pt idx="221">
-                  <c:v>6.8039999999999994</c:v>
-                </c:pt>
-                <c:pt idx="222">
-                  <c:v>6.9480000000000004</c:v>
-                </c:pt>
-                <c:pt idx="223">
-                  <c:v>11.896000000000001</c:v>
-                </c:pt>
-                <c:pt idx="224">
-                  <c:v>6.8039999999999994</c:v>
-                </c:pt>
-                <c:pt idx="225">
-                  <c:v>8.7670000000000012</c:v>
-                </c:pt>
-                <c:pt idx="226">
-                  <c:v>8.0489999999999995</c:v>
-                </c:pt>
-                <c:pt idx="227">
-                  <c:v>11.896000000000001</c:v>
-                </c:pt>
-                <c:pt idx="228">
-                  <c:v>6.8039999999999994</c:v>
-                </c:pt>
-                <c:pt idx="229">
-                  <c:v>6.9480000000000004</c:v>
-                </c:pt>
-                <c:pt idx="230">
-                  <c:v>11.896000000000001</c:v>
-                </c:pt>
-                <c:pt idx="231">
-                  <c:v>6.8039999999999994</c:v>
-                </c:pt>
-                <c:pt idx="232">
-                  <c:v>8.7670000000000012</c:v>
-                </c:pt>
-                <c:pt idx="233">
-                  <c:v>8.0489999999999995</c:v>
-                </c:pt>
-                <c:pt idx="234">
-                  <c:v>11.896000000000001</c:v>
-                </c:pt>
-                <c:pt idx="235">
-                  <c:v>6.8039999999999994</c:v>
-                </c:pt>
-                <c:pt idx="236">
-                  <c:v>6.9480000000000004</c:v>
-                </c:pt>
-                <c:pt idx="237">
-                  <c:v>11.896000000000001</c:v>
-                </c:pt>
-                <c:pt idx="238">
-                  <c:v>6.8039999999999994</c:v>
-                </c:pt>
-                <c:pt idx="239">
-                  <c:v>8.7670000000000012</c:v>
-                </c:pt>
-                <c:pt idx="240">
-                  <c:v>8.0489999999999995</c:v>
-                </c:pt>
-                <c:pt idx="241">
-                  <c:v>11.896000000000001</c:v>
-                </c:pt>
-                <c:pt idx="242">
-                  <c:v>6.8039999999999994</c:v>
-                </c:pt>
-                <c:pt idx="243">
-                  <c:v>6.9480000000000004</c:v>
-                </c:pt>
-                <c:pt idx="244">
-                  <c:v>11.896000000000001</c:v>
-                </c:pt>
-                <c:pt idx="245">
-                  <c:v>6.8039999999999994</c:v>
-                </c:pt>
-                <c:pt idx="246">
-                  <c:v>8.7670000000000012</c:v>
-                </c:pt>
-                <c:pt idx="247">
-                  <c:v>8.0489999999999995</c:v>
-                </c:pt>
-                <c:pt idx="248">
-                  <c:v>11.896000000000001</c:v>
-                </c:pt>
-                <c:pt idx="249">
-                  <c:v>6.8039999999999994</c:v>
-                </c:pt>
-                <c:pt idx="250">
-                  <c:v>7.1110000000000007</c:v>
-                </c:pt>
-                <c:pt idx="251">
-                  <c:v>15.753</c:v>
-                </c:pt>
-                <c:pt idx="252">
-                  <c:v>7.7470000000000008</c:v>
-                </c:pt>
-                <c:pt idx="253">
-                  <c:v>11.162000000000001</c:v>
-                </c:pt>
-                <c:pt idx="254">
-                  <c:v>9.8129999999999988</c:v>
-                </c:pt>
-                <c:pt idx="255">
-                  <c:v>15.753</c:v>
-                </c:pt>
-                <c:pt idx="256">
-                  <c:v>7.7470000000000008</c:v>
-                </c:pt>
-                <c:pt idx="257">
-                  <c:v>8.0549999999999997</c:v>
-                </c:pt>
-                <c:pt idx="258">
-                  <c:v>15.753</c:v>
-                </c:pt>
-                <c:pt idx="259">
-                  <c:v>7.7470000000000008</c:v>
-                </c:pt>
-                <c:pt idx="260">
-                  <c:v>11.162000000000001</c:v>
-                </c:pt>
-                <c:pt idx="261">
-                  <c:v>9.8129999999999988</c:v>
-                </c:pt>
-                <c:pt idx="262">
-                  <c:v>15.753</c:v>
-                </c:pt>
-                <c:pt idx="263">
-                  <c:v>7.7470000000000008</c:v>
-                </c:pt>
-                <c:pt idx="264">
-                  <c:v>8.0549999999999997</c:v>
-                </c:pt>
-                <c:pt idx="265">
-                  <c:v>15.753</c:v>
-                </c:pt>
-                <c:pt idx="266">
-                  <c:v>7.7470000000000008</c:v>
-                </c:pt>
-                <c:pt idx="267">
-                  <c:v>11.162000000000001</c:v>
-                </c:pt>
-                <c:pt idx="268">
-                  <c:v>9.8129999999999988</c:v>
-                </c:pt>
-                <c:pt idx="269">
-                  <c:v>15.753</c:v>
-                </c:pt>
-                <c:pt idx="270">
-                  <c:v>7.7470000000000008</c:v>
-                </c:pt>
-                <c:pt idx="271">
-                  <c:v>8.0549999999999997</c:v>
-                </c:pt>
-                <c:pt idx="272">
-                  <c:v>15.753</c:v>
-                </c:pt>
-                <c:pt idx="273">
-                  <c:v>7.7470000000000008</c:v>
-                </c:pt>
-                <c:pt idx="274">
-                  <c:v>11.162000000000001</c:v>
-                </c:pt>
-                <c:pt idx="275">
-                  <c:v>9.8129999999999988</c:v>
-                </c:pt>
-                <c:pt idx="276">
-                  <c:v>15.753</c:v>
-                </c:pt>
-                <c:pt idx="277">
-                  <c:v>7.7470000000000008</c:v>
-                </c:pt>
-                <c:pt idx="278">
-                  <c:v>8.0549999999999997</c:v>
-                </c:pt>
-                <c:pt idx="279">
-                  <c:v>15.753</c:v>
-                </c:pt>
-                <c:pt idx="280">
-                  <c:v>7.7470000000000008</c:v>
-                </c:pt>
-                <c:pt idx="281">
-                  <c:v>11.162000000000001</c:v>
-                </c:pt>
-                <c:pt idx="282">
-                  <c:v>9.8129999999999988</c:v>
-                </c:pt>
-                <c:pt idx="283">
-                  <c:v>15.753</c:v>
-                </c:pt>
-                <c:pt idx="284">
-                  <c:v>7.7470000000000008</c:v>
-                </c:pt>
-                <c:pt idx="285">
-                  <c:v>8.0549999999999997</c:v>
-                </c:pt>
-                <c:pt idx="286">
-                  <c:v>15.753</c:v>
-                </c:pt>
-                <c:pt idx="287">
-                  <c:v>7.7470000000000008</c:v>
-                </c:pt>
-                <c:pt idx="288">
-                  <c:v>11.162000000000001</c:v>
-                </c:pt>
-                <c:pt idx="289">
-                  <c:v>9.8129999999999988</c:v>
-                </c:pt>
-                <c:pt idx="290">
-                  <c:v>15.753</c:v>
-                </c:pt>
-                <c:pt idx="291">
-                  <c:v>7.7470000000000008</c:v>
-                </c:pt>
-                <c:pt idx="292">
-                  <c:v>8.0549999999999997</c:v>
-                </c:pt>
-                <c:pt idx="293">
-                  <c:v>15.753</c:v>
-                </c:pt>
-                <c:pt idx="294">
-                  <c:v>7.7470000000000008</c:v>
-                </c:pt>
-                <c:pt idx="295">
-                  <c:v>11.162000000000001</c:v>
-                </c:pt>
-                <c:pt idx="296">
-                  <c:v>9.8129999999999988</c:v>
-                </c:pt>
-                <c:pt idx="297">
-                  <c:v>15.753</c:v>
-                </c:pt>
-                <c:pt idx="298">
-                  <c:v>7.7470000000000008</c:v>
-                </c:pt>
-                <c:pt idx="299">
-                  <c:v>8.0549999999999997</c:v>
-                </c:pt>
-                <c:pt idx="300">
-                  <c:v>47.908999999999999</c:v>
-                </c:pt>
-                <c:pt idx="301">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="302">
-                  <c:v>28.382000000000001</c:v>
-                </c:pt>
-                <c:pt idx="303">
-                  <c:v>17.928999999999998</c:v>
-                </c:pt>
-                <c:pt idx="304">
-                  <c:v>47.908999999999999</c:v>
-                </c:pt>
-                <c:pt idx="305">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="306">
-                  <c:v>12.695</c:v>
-                </c:pt>
-                <c:pt idx="307">
-                  <c:v>47.908999999999999</c:v>
-                </c:pt>
-                <c:pt idx="308">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="309">
-                  <c:v>28.382000000000001</c:v>
-                </c:pt>
-                <c:pt idx="310">
-                  <c:v>17.928999999999998</c:v>
-                </c:pt>
-                <c:pt idx="311">
-                  <c:v>47.908999999999999</c:v>
-                </c:pt>
-                <c:pt idx="312">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="313">
-                  <c:v>12.695</c:v>
-                </c:pt>
-                <c:pt idx="314">
-                  <c:v>47.908999999999999</c:v>
-                </c:pt>
-                <c:pt idx="315">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="316">
-                  <c:v>28.382000000000001</c:v>
-                </c:pt>
-                <c:pt idx="317">
-                  <c:v>17.928999999999998</c:v>
-                </c:pt>
-                <c:pt idx="318">
-                  <c:v>47.908999999999999</c:v>
-                </c:pt>
-                <c:pt idx="319">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="320">
-                  <c:v>12.695</c:v>
-                </c:pt>
-                <c:pt idx="321">
-                  <c:v>47.908999999999999</c:v>
-                </c:pt>
-                <c:pt idx="322">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="323">
-                  <c:v>28.382000000000001</c:v>
-                </c:pt>
-                <c:pt idx="324">
-                  <c:v>17.928999999999998</c:v>
-                </c:pt>
-                <c:pt idx="325">
-                  <c:v>47.908999999999999</c:v>
-                </c:pt>
-                <c:pt idx="326">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="327">
-                  <c:v>12.695</c:v>
-                </c:pt>
-                <c:pt idx="328">
-                  <c:v>47.908999999999999</c:v>
-                </c:pt>
-                <c:pt idx="329">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="330">
-                  <c:v>28.382000000000001</c:v>
-                </c:pt>
-                <c:pt idx="331">
-                  <c:v>17.928999999999998</c:v>
-                </c:pt>
-                <c:pt idx="332">
-                  <c:v>47.908999999999999</c:v>
-                </c:pt>
-                <c:pt idx="333">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="334">
-                  <c:v>12.695</c:v>
-                </c:pt>
-                <c:pt idx="335">
-                  <c:v>47.908999999999999</c:v>
-                </c:pt>
-                <c:pt idx="336">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="337">
-                  <c:v>28.382000000000001</c:v>
-                </c:pt>
-                <c:pt idx="338">
-                  <c:v>17.928999999999998</c:v>
-                </c:pt>
-                <c:pt idx="339">
-                  <c:v>47.908999999999999</c:v>
-                </c:pt>
-                <c:pt idx="340">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="341">
-                  <c:v>12.695</c:v>
-                </c:pt>
-                <c:pt idx="342">
-                  <c:v>47.908999999999999</c:v>
-                </c:pt>
-                <c:pt idx="343">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="344">
-                  <c:v>28.382000000000001</c:v>
-                </c:pt>
-                <c:pt idx="345">
-                  <c:v>17.928999999999998</c:v>
-                </c:pt>
-                <c:pt idx="346">
-                  <c:v>47.908999999999999</c:v>
-                </c:pt>
-                <c:pt idx="347">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="348">
-                  <c:v>12.695</c:v>
-                </c:pt>
-                <c:pt idx="349">
-                  <c:v>47.908999999999999</c:v>
-                </c:pt>
-                <c:pt idx="350">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="351">
-                  <c:v>57.566000000000003</c:v>
-                </c:pt>
-                <c:pt idx="352">
-                  <c:v>27.992000000000001</c:v>
-                </c:pt>
-                <c:pt idx="353">
-                  <c:v>95.289000000000001</c:v>
-                </c:pt>
-                <c:pt idx="354">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="355">
-                  <c:v>19.73</c:v>
-                </c:pt>
-                <c:pt idx="356">
-                  <c:v>95.289000000000001</c:v>
-                </c:pt>
-                <c:pt idx="357">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="358">
-                  <c:v>57.566000000000003</c:v>
-                </c:pt>
-                <c:pt idx="359">
-                  <c:v>27.992000000000001</c:v>
-                </c:pt>
-                <c:pt idx="360">
-                  <c:v>95.289000000000001</c:v>
-                </c:pt>
-                <c:pt idx="361">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="362">
-                  <c:v>19.73</c:v>
-                </c:pt>
-                <c:pt idx="363">
-                  <c:v>95.289000000000001</c:v>
-                </c:pt>
-                <c:pt idx="364">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="365">
-                  <c:v>57.566000000000003</c:v>
-                </c:pt>
-                <c:pt idx="366">
-                  <c:v>27.992000000000001</c:v>
-                </c:pt>
-                <c:pt idx="367">
-                  <c:v>95.289000000000001</c:v>
-                </c:pt>
-                <c:pt idx="368">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="369">
-                  <c:v>19.73</c:v>
-                </c:pt>
-                <c:pt idx="370">
-                  <c:v>95.289000000000001</c:v>
-                </c:pt>
-                <c:pt idx="371">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="372">
-                  <c:v>57.566000000000003</c:v>
-                </c:pt>
-                <c:pt idx="373">
-                  <c:v>27.992000000000001</c:v>
-                </c:pt>
-                <c:pt idx="374">
-                  <c:v>95.289000000000001</c:v>
-                </c:pt>
-                <c:pt idx="375">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="376">
-                  <c:v>19.73</c:v>
-                </c:pt>
-                <c:pt idx="377">
-                  <c:v>95.289000000000001</c:v>
-                </c:pt>
-                <c:pt idx="378">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="379">
-                  <c:v>57.566000000000003</c:v>
-                </c:pt>
-                <c:pt idx="380">
-                  <c:v>27.992000000000001</c:v>
-                </c:pt>
-                <c:pt idx="381">
-                  <c:v>95.289000000000001</c:v>
-                </c:pt>
-                <c:pt idx="382">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="383">
-                  <c:v>19.73</c:v>
-                </c:pt>
-                <c:pt idx="384">
-                  <c:v>95.289000000000001</c:v>
-                </c:pt>
-                <c:pt idx="385">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="386">
-                  <c:v>57.566000000000003</c:v>
-                </c:pt>
-                <c:pt idx="387">
-                  <c:v>27.992000000000001</c:v>
-                </c:pt>
-                <c:pt idx="388">
-                  <c:v>95.289000000000001</c:v>
-                </c:pt>
-                <c:pt idx="389">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="390">
-                  <c:v>19.73</c:v>
-                </c:pt>
-                <c:pt idx="391">
-                  <c:v>95.289000000000001</c:v>
-                </c:pt>
-                <c:pt idx="392">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="393">
-                  <c:v>57.566000000000003</c:v>
-                </c:pt>
-                <c:pt idx="394">
-                  <c:v>27.992000000000001</c:v>
-                </c:pt>
-                <c:pt idx="395">
-                  <c:v>95.289000000000001</c:v>
-                </c:pt>
-                <c:pt idx="396">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-                <c:pt idx="397">
-                  <c:v>19.73</c:v>
-                </c:pt>
-                <c:pt idx="398">
-                  <c:v>95.289000000000001</c:v>
-                </c:pt>
-                <c:pt idx="399">
-                  <c:v>9.2799999999999994</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D71B-764F-BA8E-8B7840D13606}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="276354768"/>
-        <c:axId val="276356400"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="276354768"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="276356400"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="276356400"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-CN"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="276354768"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-CN"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="zh-CN"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="图表 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D77ED8A0-F7F7-874D-AA3C-A5991668DBF8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3946,9 +614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W401"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W1" sqref="W1:W1048576"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData>
@@ -32423,7 +29089,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -88122,10 +84787,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24:H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -88194,7 +84859,7 @@
         <v>10000</v>
       </c>
       <c r="H2">
-        <v>4.6691350363316753</v>
+        <v>4.5585377299085703</v>
       </c>
       <c r="I2">
         <v>1876</v>
@@ -88235,7 +84900,7 @@
         <v>10000</v>
       </c>
       <c r="H3">
-        <v>5.1015796661426336</v>
+        <v>4.5750288824224903</v>
       </c>
       <c r="I3">
         <v>1876</v>
@@ -88276,7 +84941,7 @@
         <v>10000</v>
       </c>
       <c r="H4">
-        <v>5.0009481855944067</v>
+        <v>4.3956359784449841</v>
       </c>
       <c r="I4">
         <v>1876</v>
@@ -88317,7 +84982,7 @@
         <v>10000</v>
       </c>
       <c r="H5">
-        <v>6.7658142061765183</v>
+        <v>4.8750175989425912</v>
       </c>
       <c r="I5">
         <v>1876</v>
@@ -88358,7 +85023,7 @@
         <v>10000</v>
       </c>
       <c r="H6">
-        <v>4.8564914786808799</v>
+        <v>4.4574551994383516</v>
       </c>
       <c r="I6">
         <v>1876</v>
@@ -88399,7 +85064,7 @@
         <v>10000</v>
       </c>
       <c r="H7">
-        <v>6.5341733865118696</v>
+        <v>5.2868997333030636</v>
       </c>
       <c r="I7">
         <v>1876</v>
@@ -88440,7 +85105,7 @@
         <v>10000</v>
       </c>
       <c r="H8">
-        <v>5.2253427315823009</v>
+        <v>4.4668629316333357</v>
       </c>
       <c r="I8">
         <v>1876</v>
@@ -88481,7 +85146,7 @@
         <v>10000</v>
       </c>
       <c r="H9">
-        <v>4.7204115501193309</v>
+        <v>4.4357685410760519</v>
       </c>
       <c r="I9">
         <v>1876</v>
@@ -88522,7 +85187,7 @@
         <v>10000</v>
       </c>
       <c r="H10">
-        <v>4.4314239396045148</v>
+        <v>4.3342007510035812</v>
       </c>
       <c r="I10">
         <v>1876</v>
@@ -88563,7 +85228,7 @@
         <v>10000</v>
       </c>
       <c r="H11">
-        <v>4.9818052443366341</v>
+        <v>4.4005371189208233</v>
       </c>
       <c r="I11">
         <v>1876</v>
@@ -88604,7 +85269,7 @@
         <v>10000</v>
       </c>
       <c r="H12">
-        <v>4.6637085827697247</v>
+        <v>4.2673818917458028</v>
       </c>
       <c r="I12">
         <v>1876</v>
@@ -88645,7 +85310,7 @@
         <v>10000</v>
       </c>
       <c r="H13">
-        <v>5.9748152590686834</v>
+        <v>5.0451436010286139</v>
       </c>
       <c r="I13">
         <v>1876</v>
@@ -88686,7 +85351,7 @@
         <v>10000</v>
       </c>
       <c r="H14">
-        <v>7.7177402643196009</v>
+        <v>5.4172325817708789</v>
       </c>
       <c r="I14">
         <v>1876</v>
@@ -88727,7 +85392,7 @@
         <v>10000</v>
       </c>
       <c r="H15">
-        <v>4.8747405710458072</v>
+        <v>4.3386916438023109</v>
       </c>
       <c r="I15">
         <v>1876</v>
@@ -88768,7 +85433,7 @@
         <v>10000</v>
       </c>
       <c r="H16">
-        <v>8.4930677718654763</v>
+        <v>5.9085565974271574</v>
       </c>
       <c r="I16">
         <v>1876</v>
@@ -88809,7 +85474,7 @@
         <v>10000</v>
       </c>
       <c r="H17">
-        <v>6.0244213964911193</v>
+        <v>4.66400568717492</v>
       </c>
       <c r="I17">
         <v>1876</v>
@@ -88850,7 +85515,7 @@
         <v>10000</v>
       </c>
       <c r="H18">
-        <v>5.7816782477062842</v>
+        <v>5.0054576973539602</v>
       </c>
       <c r="I18">
         <v>1876</v>
@@ -88891,7 +85556,7 @@
         <v>10000</v>
       </c>
       <c r="H19">
-        <v>4.5469193661752998</v>
+        <v>4.5008095999497666</v>
       </c>
       <c r="I19">
         <v>1876</v>
@@ -88932,7 +85597,7 @@
         <v>10000</v>
       </c>
       <c r="H20">
-        <v>5.3212654258644152</v>
+        <v>4.6154051436466554</v>
       </c>
       <c r="I20">
         <v>1876</v>
@@ -88973,7 +85638,7 @@
         <v>10000</v>
       </c>
       <c r="H21">
-        <v>4.1882005745307849</v>
+        <v>4.3449908808880124</v>
       </c>
       <c r="I21">
         <v>1876</v>
@@ -88994,22 +85659,16 @@
         <v>2.453129842683146</v>
       </c>
     </row>
+    <row r="24" spans="2:14">
+      <c r="H24">
+        <f>AVERAGE(H2:H21)</f>
+        <v>4.6946809894940937</v>
+      </c>
+    </row>
     <row r="25" spans="2:14">
       <c r="H25">
-        <f>AVERAGE(H2:H21)</f>
-        <v>5.493684144245897</v>
-      </c>
-    </row>
-    <row r="26" spans="2:14">
-      <c r="H26">
         <f>STDEV(H2:H21)</f>
-        <v>1.1352000691444177</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14">
-      <c r="H27">
-        <f>MIN(H2:H21)</f>
-        <v>4.1882005745307849</v>
+        <v>0.43459552506079241</v>
       </c>
     </row>
   </sheetData>

</xml_diff>